<commit_message>
Add a couple more tableau alias sheets
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7F9015-1D71-4732-8210-E0C6EDB892EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFDE0C0-4F89-4DAC-951F-726584118722}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20955" yWindow="1620" windowWidth="19170" windowHeight="11970" activeTab="2" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="14220" yWindow="600" windowWidth="23040" windowHeight="14685" activeTab="4" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
     <sheet name="Tour Mode" sheetId="2" r:id="rId2"/>
     <sheet name="Person Type" sheetId="3" r:id="rId3"/>
+    <sheet name="Facility Type" sheetId="4" r:id="rId4"/>
+    <sheet name="Area Type" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -138,13 +140,73 @@
   </si>
   <si>
     <t>College student</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>Freeway-to-freeway connector</t>
+  </si>
+  <si>
+    <t>Freeway</t>
+  </si>
+  <si>
+    <t>Expressway</t>
+  </si>
+  <si>
+    <t>Collector</t>
+  </si>
+  <si>
+    <t>Freeway ramp</t>
+  </si>
+  <si>
+    <t>Dummy link</t>
+  </si>
+  <si>
+    <t>Major arterial</t>
+  </si>
+  <si>
+    <t>Managed Freeway</t>
+  </si>
+  <si>
+    <t>Special facility</t>
+  </si>
+  <si>
+    <t>Toll plaza</t>
+  </si>
+  <si>
+    <t>FacilityType</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>Regional core</t>
+  </si>
+  <si>
+    <t>Central business district</t>
+  </si>
+  <si>
+    <t>Urban business</t>
+  </si>
+  <si>
+    <t>Urban</t>
+  </si>
+  <si>
+    <t>Suburban</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>AreaType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +223,26 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -206,6 +288,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -408,6 +517,166 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2647950" y="466725"/>
+          <a:ext cx="6266587" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>For blending with data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> in Tableau</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>see </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>https://help.tableau.com/v2018.3/pro/desktop/en-us/multipleconnections_edit_primary_aliases.htm</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6266587" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EAE6F3B-B84E-4540-8346-10794FBE4DEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3028950" y="400050"/>
+          <a:ext cx="6266587" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>For blending with data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> in Tableau</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>see </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>https://help.tableau.com/v2018.3/pro/desktop/en-us/multipleconnections_edit_primary_aliases.htm</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6266587" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B3CFCE5-008A-4565-95B0-276994906D89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2867025" y="400050"/>
           <a:ext cx="6266587" cy="436786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1155,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DDFD75-CDE7-458C-A68B-27F57FAFDC8F}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,4 +1562,204 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C72F0B4-5112-44C4-A154-2365DFF42B7C}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511536D8-7156-4B5A-99A3-DBFB1C8D0C5A}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Utilities updates - mainly paths and some more tableau aliases
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFDE0C0-4F89-4DAC-951F-726584118722}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F365C842-198F-48A4-8403-8EB480437F3F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14220" yWindow="600" windowWidth="23040" windowHeight="14685" activeTab="4" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="375" yWindow="360" windowWidth="20400" windowHeight="14640" activeTab="5" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Person Type" sheetId="3" r:id="rId3"/>
     <sheet name="Facility Type" sheetId="4" r:id="rId4"/>
     <sheet name="Area Type" sheetId="5" r:id="rId5"/>
+    <sheet name="County" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -200,13 +201,49 @@
   </si>
   <si>
     <t>AreaType</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>County Name</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>San Mateo</t>
+  </si>
+  <si>
+    <t>Santa Clara</t>
+  </si>
+  <si>
+    <t>Alameda</t>
+  </si>
+  <si>
+    <t>Contra Costa</t>
+  </si>
+  <si>
+    <t>Solano</t>
+  </si>
+  <si>
+    <t>Napa</t>
+  </si>
+  <si>
+    <t>Sonoma</t>
+  </si>
+  <si>
+    <t>Marin</t>
+  </si>
+  <si>
+    <t>External to Bay Area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +284,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -277,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -316,6 +361,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1676,7 +1733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511536D8-7156-4B5A-99A3-DBFB1C8D0C5A}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1762,4 +1819,110 @@
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9A15B5-579C-442B-8039-6B78A1A82839}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="13" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a missing transit mode to TableauAliases.xlsx
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1D7855-672B-45AB-B53D-9BEB8CC0B514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451DDC2B-EF85-431D-B54B-386401CB4D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="4755" windowWidth="19230" windowHeight="14640" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="1965" yWindow="6615" windowWidth="20085" windowHeight="12615" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="County" sheetId="6" r:id="rId6"/>
     <sheet name="Transit Mode" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="161">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -423,9 +423,6 @@
     <t>SMART - Temporary Express</t>
   </si>
   <si>
-    <t>Regional Express ReX Express Routes (PPA Project) - Express</t>
-  </si>
-  <si>
     <t>East Bay Ferries</t>
   </si>
   <si>
@@ -514,6 +511,15 @@
   </si>
   <si>
     <t>Transit Mode</t>
+  </si>
+  <si>
+    <t>Dumbarton Group Rapid Transit (GRT)</t>
+  </si>
+  <si>
+    <t>VINE - Express 2</t>
+  </si>
+  <si>
+    <t>Regional Express (ReX)</t>
   </si>
 </sst>
 </file>
@@ -2282,11 +2288,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2297,18 +2303,18 @@
     <col min="4" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -2319,7 +2325,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="20">
         <v>2</v>
       </c>
@@ -2330,7 +2336,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>3</v>
       </c>
@@ -2341,7 +2347,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>4</v>
       </c>
@@ -2352,7 +2358,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>5</v>
       </c>
@@ -2363,7 +2369,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>6</v>
       </c>
@@ -2374,7 +2380,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>7</v>
       </c>
@@ -2385,7 +2391,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
         <v>10</v>
       </c>
@@ -2396,7 +2402,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
         <v>11</v>
       </c>
@@ -2407,7 +2413,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
         <v>12</v>
       </c>
@@ -2418,7 +2424,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>13</v>
       </c>
@@ -2429,7 +2435,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>14</v>
       </c>
@@ -2440,7 +2446,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
         <v>15</v>
       </c>
@@ -2451,7 +2457,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
         <v>16</v>
       </c>
@@ -2462,7 +2468,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
         <v>17</v>
       </c>
@@ -2473,7 +2479,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="20">
         <v>18</v>
       </c>
@@ -2484,7 +2490,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="20">
         <v>19</v>
       </c>
@@ -2495,7 +2501,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="20">
         <v>20</v>
       </c>
@@ -2506,7 +2512,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="20">
         <v>21</v>
       </c>
@@ -2517,7 +2523,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="20">
         <v>24</v>
       </c>
@@ -2528,7 +2534,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="20">
         <v>27</v>
       </c>
@@ -2539,7 +2545,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="20">
         <v>28</v>
       </c>
@@ -2550,7 +2556,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>30</v>
       </c>
@@ -2561,7 +2567,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>33</v>
       </c>
@@ -2572,7 +2578,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="20">
         <v>38</v>
       </c>
@@ -2583,7 +2589,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="20">
         <v>42</v>
       </c>
@@ -2594,7 +2600,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="20">
         <v>44</v>
       </c>
@@ -2605,7 +2611,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="20">
         <v>46</v>
       </c>
@@ -2616,7 +2622,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="20">
         <v>49</v>
       </c>
@@ -2627,7 +2633,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="20">
         <v>52</v>
       </c>
@@ -2638,7 +2644,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="20">
         <v>55</v>
       </c>
@@ -2649,7 +2655,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="20">
         <v>56</v>
       </c>
@@ -2660,7 +2666,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="20">
         <v>58</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="20">
         <v>60</v>
       </c>
@@ -2682,7 +2688,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="20">
         <v>63</v>
       </c>
@@ -2693,7 +2699,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="20">
         <v>66</v>
       </c>
@@ -2704,7 +2710,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="20">
         <v>68</v>
       </c>
@@ -2715,7 +2721,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="20">
         <v>69</v>
       </c>
@@ -2726,7 +2732,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="20">
         <v>70</v>
       </c>
@@ -2737,7 +2743,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="20">
         <v>75</v>
       </c>
@@ -2748,7 +2754,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="20">
         <v>78</v>
       </c>
@@ -2759,7 +2765,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="20">
         <v>80</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="20">
         <v>81</v>
       </c>
@@ -2781,7 +2787,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="20">
         <v>82</v>
       </c>
@@ -2792,7 +2798,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="20">
         <v>83</v>
       </c>
@@ -2803,7 +2809,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="20">
         <v>84</v>
       </c>
@@ -2814,7 +2820,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="20">
         <v>85</v>
       </c>
@@ -2825,7 +2831,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="20">
         <v>86</v>
       </c>
@@ -2836,7 +2842,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="20">
         <v>87</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="20">
         <v>88</v>
       </c>
@@ -2858,7 +2864,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="20">
         <v>89</v>
       </c>
@@ -2869,7 +2875,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="20">
         <v>90</v>
       </c>
@@ -2880,7 +2886,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="20">
         <v>91</v>
       </c>
@@ -2891,7 +2897,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="20">
         <v>92</v>
       </c>
@@ -2902,7 +2908,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="20">
         <v>93</v>
       </c>
@@ -2913,7 +2919,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="20">
         <v>94</v>
       </c>
@@ -2924,290 +2930,301 @@
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="20">
         <v>95</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="20">
         <v>98</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="C59" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="20">
         <v>100</v>
       </c>
       <c r="B60" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C60" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C60" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="20">
         <v>101</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="20">
         <v>102</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="20">
         <v>103</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="20">
         <v>104</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="20">
         <v>105</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="20">
         <v>106</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="20">
         <v>110</v>
       </c>
       <c r="B67" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C67" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="20">
         <v>111</v>
       </c>
       <c r="B68" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="20">
+        <v>112</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="20">
+        <v>113</v>
+      </c>
+      <c r="B70" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="C68" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="20">
-        <v>113</v>
-      </c>
-      <c r="B69" s="20" t="s">
+      <c r="C70" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="20">
+        <v>114</v>
+      </c>
+      <c r="B71" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="20">
-        <v>114</v>
-      </c>
-      <c r="B70" s="20" t="s">
+      <c r="C71" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="20">
+        <v>115</v>
+      </c>
+      <c r="B72" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="20">
-        <v>115</v>
-      </c>
-      <c r="B71" s="20" t="s">
+      <c r="C72" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="20">
+        <v>116</v>
+      </c>
+      <c r="B73" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="C71" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="20">
-        <v>116</v>
-      </c>
-      <c r="B72" s="20" t="s">
+      <c r="C73" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="20">
+        <v>117</v>
+      </c>
+      <c r="B74" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="C72" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="20">
-        <v>117</v>
-      </c>
-      <c r="B73" s="20" t="s">
+      <c r="C74" s="20" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="20">
+        <v>120</v>
+      </c>
+      <c r="B75" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="C73" s="20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="20">
-        <v>120</v>
-      </c>
-      <c r="B74" s="20" t="s">
+      <c r="C75" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="C74" s="20" t="s">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="20">
+        <v>121</v>
+      </c>
+      <c r="B76" s="20" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="20">
-        <v>121</v>
-      </c>
-      <c r="B75" s="20" t="s">
+      <c r="C76" s="20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="20">
+        <v>130</v>
+      </c>
+      <c r="B77" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="C75" s="20" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="20">
-        <v>130</v>
-      </c>
-      <c r="B76" s="20" t="s">
+      <c r="C77" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="C76" s="20" t="s">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="20">
+        <v>131</v>
+      </c>
+      <c r="B78" s="20" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="20">
-        <v>131</v>
-      </c>
-      <c r="B77" s="20" t="s">
+      <c r="C78" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="20">
+        <v>132</v>
+      </c>
+      <c r="B79" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="C77" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="20">
-        <v>132</v>
-      </c>
-      <c r="B78" s="20" t="s">
+      <c r="C79" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="20">
+        <v>133</v>
+      </c>
+      <c r="B80" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="C78" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="20">
-        <v>133</v>
-      </c>
-      <c r="B79" s="20" t="s">
+      <c r="C80" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="20">
+        <v>134</v>
+      </c>
+      <c r="B81" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="C79" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="20">
-        <v>134</v>
-      </c>
-      <c r="B80" s="20" t="s">
+      <c r="C81" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="20">
+        <v>135</v>
+      </c>
+      <c r="B82" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="C80" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="20">
-        <v>135</v>
-      </c>
-      <c r="B81" s="20" t="s">
+      <c r="C82" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="20">
+        <v>136</v>
+      </c>
+      <c r="B83" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="C81" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="20">
-        <v>136</v>
-      </c>
-      <c r="B82" s="20" t="s">
+      <c r="C83" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="20">
+        <v>137</v>
+      </c>
+      <c r="B84" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="C82" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="20">
-        <v>137</v>
-      </c>
-      <c r="B83" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C83" s="20" t="s">
-        <v>149</v>
+      <c r="C84" s="20" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Common.Agency.Name mapping for transit modes
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451DDC2B-EF85-431D-B54B-386401CB4D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B29285F-1012-43D7-9632-F4FA696E80ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="6615" windowWidth="20085" windowHeight="12615" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="14940" yWindow="1695" windowWidth="21330" windowHeight="12900" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="County" sheetId="6" r:id="rId6"/>
     <sheet name="Transit Mode" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="178">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -520,6 +525,57 @@
   </si>
   <si>
     <t>Regional Express (ReX)</t>
+  </si>
+  <si>
+    <t>Common.Agency.Name</t>
+  </si>
+  <si>
+    <t>Other Transit Agencies</t>
+  </si>
+  <si>
+    <t>VTA</t>
+  </si>
+  <si>
+    <t>LAVTA</t>
+  </si>
+  <si>
+    <t>SFMTA</t>
+  </si>
+  <si>
+    <t>SamTrans</t>
+  </si>
+  <si>
+    <t>AC Transit</t>
+  </si>
+  <si>
+    <t>County Connection</t>
+  </si>
+  <si>
+    <t>Tri Delta Transit</t>
+  </si>
+  <si>
+    <t>WestCAT</t>
+  </si>
+  <si>
+    <t>SolTrans</t>
+  </si>
+  <si>
+    <t>FAST</t>
+  </si>
+  <si>
+    <t>Napa VINE</t>
+  </si>
+  <si>
+    <t>Marin Transit</t>
+  </si>
+  <si>
+    <t>GGBHTD</t>
+  </si>
+  <si>
+    <t>WETA</t>
+  </si>
+  <si>
+    <t>BART</t>
   </si>
 </sst>
 </file>
@@ -612,40 +668,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -655,10 +711,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1085,12 +1137,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4847161" cy="264560"/>
+    <xdr:ext cx="4847161" cy="609013"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -1104,8 +1156,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6286500" y="561975"/>
-          <a:ext cx="4847161" cy="264560"/>
+          <a:off x="7381875" y="390525"/>
+          <a:ext cx="4847161" cy="609013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1133,14 +1185,35 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>Source: https://github.com/BayAreaMetro/modeling-website/wiki/TransitModes</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> </a:t>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Common.Agency.Name is useful for NTD </a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2193,10 +2266,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2209,74 +2282,74 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2288,943 +2361,1196 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="61.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="12.85546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="61.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="18" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="20">
+      <c r="D1" s="18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="20">
+      <c r="D2" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="20">
+      <c r="D3" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="20">
+      <c r="D4" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="20">
+      <c r="D5" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="20">
+      <c r="D6" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="20">
+      <c r="D7" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="20">
+      <c r="D8" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
         <v>10</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
+      <c r="D9" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
         <v>11</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="20">
+      <c r="D10" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
         <v>12</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="20">
+      <c r="D11" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
         <v>13</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="20">
+      <c r="D12" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
         <v>14</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="20">
+      <c r="D13" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
         <v>15</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="20">
+      <c r="D14" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
         <v>16</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="20">
+      <c r="D15" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
         <v>17</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="20">
+      <c r="D16" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
         <v>18</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="20">
+      <c r="D17" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
         <v>19</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="20">
+      <c r="D18" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
         <v>20</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="20">
+      <c r="D19" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
         <v>21</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="20">
+      <c r="D20" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="18">
         <v>24</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="20">
+      <c r="D21" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="18">
         <v>27</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="20">
+      <c r="D22" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="18">
         <v>28</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="20">
+      <c r="D23" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="18">
         <v>30</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="20">
+      <c r="D24" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
         <v>33</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="20">
+      <c r="D25" s="18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="18">
         <v>38</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="20">
+      <c r="D26" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="18">
         <v>42</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="20">
+      <c r="D27" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="18">
         <v>44</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="20">
+      <c r="D28" s="18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="18">
         <v>46</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="20">
+      <c r="D29" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="18">
         <v>49</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="20">
+      <c r="D30" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="18">
         <v>52</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="20">
+      <c r="D31" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="18">
         <v>55</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="20">
+      <c r="D32" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="18">
         <v>56</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="20">
+      <c r="D33" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="18">
         <v>58</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="20">
+      <c r="D34" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="18">
         <v>60</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="20">
+      <c r="D35" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="18">
         <v>63</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="20">
+      <c r="D36" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="18">
         <v>66</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="20">
+      <c r="D37" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="18">
         <v>68</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="20">
+      <c r="D38" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="18">
         <v>69</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="20">
+      <c r="D39" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="18">
         <v>70</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="20">
+      <c r="D40" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="18">
         <v>75</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="20">
+      <c r="D41" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="18">
         <v>78</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="20">
+      <c r="D42" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="18">
         <v>80</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="20">
+      <c r="D43" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="18">
         <v>81</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="20" t="s">
+      <c r="C44" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="20">
+      <c r="D44" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="18">
         <v>82</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="20">
+      <c r="D45" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="18">
         <v>83</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="20">
+      <c r="D46" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="18">
         <v>84</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="20">
+      <c r="D47" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="18">
         <v>85</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="18" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="20">
+      <c r="D48" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="18">
         <v>86</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="20">
+      <c r="D49" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="18">
         <v>87</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="20">
+      <c r="D50" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="18">
         <v>88</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="20">
+      <c r="D51" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="18">
         <v>89</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="20" t="s">
+      <c r="C52" s="18" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="20">
+      <c r="D52" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="18">
         <v>90</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="20">
+      <c r="D53" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="18">
         <v>91</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="20">
+      <c r="D54" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="18">
         <v>92</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="20">
+      <c r="D55" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="18">
         <v>93</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="20">
+      <c r="D56" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="18">
         <v>94</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="20">
+      <c r="D57" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="18">
         <v>95</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="20">
+      <c r="D58" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="18">
         <v>98</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="20">
+      <c r="D59" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="18">
         <v>100</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C60" s="18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="20">
+      <c r="D60" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="18">
         <v>101</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="20">
+      <c r="D61" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="18">
         <v>102</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="20">
+      <c r="D62" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="18">
         <v>103</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="20">
+      <c r="D63" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="18">
         <v>104</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="20">
+      <c r="D64" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="18">
         <v>105</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="20">
+      <c r="D65" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="18">
         <v>106</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="20">
+      <c r="D66" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="18">
         <v>110</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="20">
+      <c r="D67" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="18">
         <v>111</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="20">
+      <c r="D68" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="18">
         <v>112</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="20">
+      <c r="D69" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="18">
         <v>113</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="20">
+      <c r="D70" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="18">
         <v>114</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="20">
+      <c r="D71" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="18">
         <v>115</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="20">
+      <c r="D72" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="18">
         <v>116</v>
       </c>
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="20">
+      <c r="D73" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="18">
         <v>117</v>
       </c>
-      <c r="B74" s="20" t="s">
+      <c r="B74" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="C74" s="20" t="s">
+      <c r="C74" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="20">
+      <c r="D74" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="18">
         <v>120</v>
       </c>
-      <c r="B75" s="20" t="s">
+      <c r="B75" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="18" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="20">
+      <c r="D75" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="18">
         <v>121</v>
       </c>
-      <c r="B76" s="20" t="s">
+      <c r="B76" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="18" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="20">
+      <c r="D76" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="18">
         <v>130</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="18" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="20">
+      <c r="D77" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="18">
         <v>131</v>
       </c>
-      <c r="B78" s="20" t="s">
+      <c r="B78" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="18" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="20">
+      <c r="D78" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="18">
         <v>132</v>
       </c>
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="18" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="20">
+      <c r="D79" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="18">
         <v>133</v>
       </c>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="C80" s="20" t="s">
+      <c r="C80" s="18" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="20">
+      <c r="D80" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="18">
         <v>134</v>
       </c>
-      <c r="B81" s="20" t="s">
+      <c r="B81" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="C81" s="20" t="s">
+      <c r="C81" s="18" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="20">
+      <c r="D81" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="18">
         <v>135</v>
       </c>
-      <c r="B82" s="20" t="s">
+      <c r="B82" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="C82" s="20" t="s">
+      <c r="C82" s="18" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="20">
+      <c r="D82" s="18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="18">
         <v>136</v>
       </c>
-      <c r="B83" s="20" t="s">
+      <c r="B83" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="C83" s="20" t="s">
+      <c r="C83" s="18" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="20">
+      <c r="D83" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="18">
         <v>137</v>
       </c>
-      <c r="B84" s="20" t="s">
+      <c r="B84" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="C84" s="20" t="s">
+      <c r="C84" s="18" t="s">
         <v>148</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Common.Agency.Name for transit modes
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B29285F-1012-43D7-9632-F4FA696E80ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5D06D0-EACE-4B13-9ABB-FF2A7B3D1A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="1695" windowWidth="21330" windowHeight="12900" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="4665" yWindow="5295" windowWidth="28800" windowHeight="17235" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="181">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -576,6 +576,15 @@
   </si>
   <si>
     <t>BART</t>
+  </si>
+  <si>
+    <t>Sonoma County Transit</t>
+  </si>
+  <si>
+    <t>Vacaville City Coach*</t>
+  </si>
+  <si>
+    <t>Union City Transit*</t>
   </si>
 </sst>
 </file>
@@ -2365,7 +2374,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2393,430 +2402,430 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
-        <v>6</v>
+        <v>133</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>69</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>77</v>
@@ -2827,10 +2836,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>77</v>
@@ -2841,10 +2850,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>77</v>
@@ -2855,24 +2864,24 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>77</v>
@@ -2883,41 +2892,41 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>106</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>162</v>
@@ -2925,27 +2934,27 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>162</v>
@@ -2953,13 +2962,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>162</v>
@@ -2967,593 +2976,596 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="18">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>116</v>
+        <v>143</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>121</v>
+        <v>154</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>112</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>173</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>159</v>
+        <v>88</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="18">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="18">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="18">
+        <v>58</v>
+      </c>
+      <c r="B62" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B62" s="18" t="s">
-        <v>131</v>
-      </c>
       <c r="C62" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="18">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="18">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="18">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
-        <v>110</v>
+        <v>2</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>136</v>
+        <v>70</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>165</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
-        <v>111</v>
+        <v>3</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>138</v>
+        <v>71</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
-        <v>113</v>
+        <v>5</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>139</v>
+        <v>73</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="18">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>140</v>
+        <v>74</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>137</v>
+        <v>69</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
-        <v>116</v>
+        <v>44</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
-        <v>117</v>
+        <v>38</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
-        <v>121</v>
+        <v>15</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="18">
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>147</v>
+        <v>90</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="18">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="18">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="18">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="18">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>152</v>
+        <v>97</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="18">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="18">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="18">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D84">
+    <sortCondition ref="D1:D84"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Create NTD files in model-style formats
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one-transit-calib-2020\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5D06D0-EACE-4B13-9ABB-FF2A7B3D1A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4A2325-F6FE-4EC0-9023-4BB7B8930751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="5295" windowWidth="28800" windowHeight="17235" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="8025" yWindow="2085" windowWidth="22785" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="192">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -563,9 +563,6 @@
     <t>FAST</t>
   </si>
   <si>
-    <t>Napa VINE</t>
-  </si>
-  <si>
     <t>Marin Transit</t>
   </si>
   <si>
@@ -585,6 +582,42 @@
   </si>
   <si>
     <t>Union City Transit*</t>
+  </si>
+  <si>
+    <t>Santa Rosa CityBus</t>
+  </si>
+  <si>
+    <t>NTD.mode</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Napa Vine</t>
   </si>
 </sst>
 </file>
@@ -1146,10 +1179,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4847161" cy="609013"/>
     <xdr:sp macro="" textlink="">
@@ -1165,7 +1198,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7381875" y="390525"/>
+          <a:off x="8924925" y="266700"/>
           <a:ext cx="4847161" cy="609013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1216,7 +1249,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Common.Agency.Name is useful for NTD </a:t>
+            <a:t>Common.Agency.Name and NTD.mode is useful for NTD  correspondence</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -2370,11 +2403,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2386,7 +2419,7 @@
     <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>157</v>
       </c>
@@ -2399,8 +2432,11 @@
       <c r="D1" s="18" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>30</v>
       </c>
@@ -2413,8 +2449,11 @@
       <c r="D2" s="18" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>82</v>
       </c>
@@ -2427,8 +2466,11 @@
       <c r="D3" s="18" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>83</v>
       </c>
@@ -2441,8 +2483,11 @@
       <c r="D4" s="18" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>84</v>
       </c>
@@ -2455,8 +2500,11 @@
       <c r="D5" s="18" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>85</v>
       </c>
@@ -2469,8 +2517,11 @@
       <c r="D6" s="18" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>133</v>
       </c>
@@ -2483,8 +2534,11 @@
       <c r="D7" s="18" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>120</v>
       </c>
@@ -2495,10 +2549,13 @@
         <v>145</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>121</v>
       </c>
@@ -2509,10 +2566,13 @@
         <v>145</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>130</v>
       </c>
@@ -2525,8 +2585,11 @@
       <c r="D10" s="18" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>42</v>
       </c>
@@ -2539,8 +2602,11 @@
       <c r="D11" s="18" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>86</v>
       </c>
@@ -2553,8 +2619,11 @@
       <c r="D12" s="18" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>52</v>
       </c>
@@ -2567,8 +2636,11 @@
       <c r="D13" s="18" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>92</v>
       </c>
@@ -2581,8 +2653,11 @@
       <c r="D14" s="18" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>87</v>
       </c>
@@ -2593,10 +2668,13 @@
         <v>112</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>88</v>
       </c>
@@ -2607,10 +2685,13 @@
         <v>112</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>101</v>
       </c>
@@ -2621,10 +2702,13 @@
         <v>129</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>102</v>
       </c>
@@ -2635,10 +2719,13 @@
         <v>129</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>103</v>
       </c>
@@ -2649,10 +2736,13 @@
         <v>129</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>17</v>
       </c>
@@ -2665,8 +2755,11 @@
       <c r="D20" s="18" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>33</v>
       </c>
@@ -2679,8 +2772,11 @@
       <c r="D21" s="18" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>70</v>
       </c>
@@ -2691,10 +2787,13 @@
         <v>77</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>60</v>
       </c>
@@ -2705,10 +2804,13 @@
         <v>77</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>93</v>
       </c>
@@ -2719,10 +2821,13 @@
         <v>112</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>95</v>
       </c>
@@ -2733,10 +2838,13 @@
         <v>112</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>55</v>
       </c>
@@ -2747,10 +2855,13 @@
         <v>77</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>10</v>
       </c>
@@ -2764,7 +2875,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>11</v>
       </c>
@@ -2778,7 +2889,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>12</v>
       </c>
@@ -2792,7 +2903,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>13</v>
       </c>
@@ -2806,7 +2917,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>14</v>
       </c>
@@ -2820,7 +2931,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>16</v>
       </c>
@@ -3058,7 +3169,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>132</v>
       </c>
@@ -3072,7 +3183,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
         <v>134</v>
       </c>
@@ -3086,7 +3197,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>136</v>
       </c>
@@ -3100,7 +3211,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <v>137</v>
       </c>
@@ -3114,7 +3225,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
         <v>68</v>
       </c>
@@ -3127,8 +3238,11 @@
       <c r="D53" s="18" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
         <v>24</v>
       </c>
@@ -3141,8 +3255,11 @@
       <c r="D54" s="18" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
         <v>80</v>
       </c>
@@ -3155,8 +3272,11 @@
       <c r="D55" s="18" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
         <v>66</v>
       </c>
@@ -3167,10 +3287,13 @@
         <v>77</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
         <v>20</v>
       </c>
@@ -3183,8 +3306,11 @@
       <c r="D57" s="18" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57" s="18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
         <v>21</v>
       </c>
@@ -3197,8 +3323,11 @@
       <c r="D58" s="18" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="18">
         <v>89</v>
       </c>
@@ -3211,8 +3340,11 @@
       <c r="D59" s="18" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="18">
         <v>110</v>
       </c>
@@ -3225,8 +3357,11 @@
       <c r="D60" s="18" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
         <v>135</v>
       </c>
@@ -3239,8 +3374,11 @@
       <c r="D61" s="18" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="18">
         <v>58</v>
       </c>
@@ -3253,8 +3391,11 @@
       <c r="D62" s="18" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="18">
         <v>49</v>
       </c>
@@ -3267,8 +3408,11 @@
       <c r="D63" s="18" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
         <v>91</v>
       </c>
@@ -3281,8 +3425,11 @@
       <c r="D64" s="18" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="18">
         <v>63</v>
       </c>
@@ -3293,10 +3440,13 @@
         <v>77</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="E65" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="18">
         <v>1</v>
       </c>
@@ -3310,7 +3460,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
         <v>2</v>
       </c>
@@ -3324,7 +3474,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
         <v>3</v>
       </c>
@@ -3338,7 +3488,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
         <v>4</v>
       </c>
@@ -3352,7 +3502,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
         <v>5</v>
       </c>
@@ -3366,7 +3516,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="18">
         <v>6</v>
       </c>
@@ -3380,7 +3530,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
         <v>7</v>
       </c>
@@ -3394,7 +3544,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
         <v>44</v>
       </c>
@@ -3407,8 +3557,11 @@
       <c r="D73" s="18" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
         <v>38</v>
       </c>
@@ -3419,10 +3572,13 @@
         <v>77</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
         <v>56</v>
       </c>
@@ -3433,10 +3589,13 @@
         <v>77</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+      <c r="E75" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
         <v>15</v>
       </c>
@@ -3449,8 +3608,11 @@
       <c r="D76" s="18" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="18">
         <v>27</v>
       </c>
@@ -3463,8 +3625,11 @@
       <c r="D77" s="18" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="18">
         <v>28</v>
       </c>
@@ -3477,8 +3642,11 @@
       <c r="D78" s="18" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="18">
         <v>81</v>
       </c>
@@ -3491,8 +3659,11 @@
       <c r="D79" s="18" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="18">
         <v>111</v>
       </c>
@@ -3505,8 +3676,11 @@
       <c r="D80" s="18" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="18">
         <v>46</v>
       </c>
@@ -3519,8 +3693,11 @@
       <c r="D81" s="18" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="18">
         <v>90</v>
       </c>
@@ -3533,8 +3710,11 @@
       <c r="D82" s="18" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="18">
         <v>100</v>
       </c>
@@ -3545,10 +3725,13 @@
         <v>129</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="18">
         <v>104</v>
       </c>
@@ -3559,11 +3742,14 @@
         <v>129</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+      <c r="E84" s="18" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D84">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
     <sortCondition ref="D1:D84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Investigate express bus differences in model vs NTD
I believe the issue is that NTD does not necessarily distinguish between express bus and local service the way our model lines do.  The NTD modes (added in NTD-mode-lookup.csv) includes CB=Commuter Bus, but not all operators that run buses that we code as express buses have that mode. So when comparing model vs NTD supply and demand, Express & Local bus modes should be collapsed.
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one-transit-calib-2020\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one-v1.6_develop\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4A2325-F6FE-4EC0-9023-4BB7B8930751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCC442B-0D1B-4842-82F2-9DF9B7EA09A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8025" yWindow="2085" windowWidth="22785" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="285" yWindow="2175" windowWidth="28800" windowHeight="15435" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="County" sheetId="6" r:id="rId6"/>
     <sheet name="Transit Mode" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Transit Mode'!$A$1:$E$84</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2407,7 +2410,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2438,254 +2441,215 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>182</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>114</v>
+        <v>70</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>183</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
-        <v>83</v>
+        <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>182</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>182</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>184</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>151</v>
+        <v>74</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>145</v>
+        <v>69</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>186</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
-        <v>130</v>
+        <v>11</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
-        <v>87</v>
+        <v>16</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>182</v>
@@ -2693,67 +2657,61 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
-        <v>103</v>
+        <v>20</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>182</v>
@@ -2761,16 +2719,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>182</v>
@@ -2778,16 +2736,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>182</v>
@@ -2795,16 +2753,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>182</v>
@@ -2812,50 +2770,50 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>159</v>
+        <v>93</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>182</v>
@@ -2863,892 +2821,942 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>162</v>
+        <v>168</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>162</v>
+        <v>169</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>162</v>
+        <v>170</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>162</v>
+        <v>171</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>162</v>
+        <v>172</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
+        <v>80</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="18">
+        <v>81</v>
+      </c>
+      <c r="B44" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="18">
+      <c r="C44" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="18">
+        <v>82</v>
+      </c>
+      <c r="B45" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="18">
+      <c r="C45" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="18">
+        <v>83</v>
+      </c>
+      <c r="B46" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B45" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="18">
+      <c r="C46" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="18">
+        <v>84</v>
+      </c>
+      <c r="B47" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="18">
+      <c r="C47" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="18">
+        <v>85</v>
+      </c>
+      <c r="B48" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="18">
-        <v>131</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="C48" s="18" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>162</v>
+        <v>167</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>162</v>
+        <v>168</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>162</v>
+        <v>174</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>162</v>
+        <v>174</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>162</v>
+        <v>165</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>112</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E57" s="18" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="18">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="18">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E59" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="18">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="18">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="18">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="C62" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="18">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="18">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="C64" s="18" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="18">
-        <v>63</v>
+        <v>105</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="E65" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="18">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
-        <v>2</v>
+        <v>110</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>69</v>
+        <v>165</v>
+      </c>
+      <c r="E67" s="18" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>69</v>
+        <v>163</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>72</v>
+        <v>158</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
-        <v>5</v>
+        <v>113</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="18">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>96</v>
+        <v>142</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="E73" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
-        <v>38</v>
+        <v>117</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="E74" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="18">
-        <v>27</v>
+        <v>130</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="18">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>91</v>
+        <v>149</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E78" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="18">
-        <v>81</v>
+        <v>132</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E79" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="18">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="E80" s="18" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="18">
-        <v>46</v>
+        <v>134</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="E81" s="18" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="18">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="18">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="E83" s="18" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="18">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="E84" s="18" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E84" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
+      <sortCondition ref="A1:A84"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
     <sortCondition ref="D1:D84"/>
   </sortState>

</xml_diff>

<commit_message>
Revert "Merge pull request #62 from BayAreaMetro/v1.6_develop"
This reverts commit 6dd723bffcd4a3e9466c02adad8486c31d18a405, reversing
changes made to fb711c06e466314c4539d3d720680b85f852f8bb.
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one-v1.6_develop\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCC442B-0D1B-4842-82F2-9DF9B7EA09A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5D06D0-EACE-4B13-9ABB-FF2A7B3D1A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="2175" windowWidth="28800" windowHeight="15435" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="4665" yWindow="5295" windowWidth="28800" windowHeight="17235" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
     <sheet name="County" sheetId="6" r:id="rId6"/>
     <sheet name="Transit Mode" sheetId="7" r:id="rId7"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Transit Mode'!$A$1:$E$84</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="181">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -566,6 +563,9 @@
     <t>FAST</t>
   </si>
   <si>
+    <t>Napa VINE</t>
+  </si>
+  <si>
     <t>Marin Transit</t>
   </si>
   <si>
@@ -585,42 +585,6 @@
   </si>
   <si>
     <t>Union City Transit*</t>
-  </si>
-  <si>
-    <t>Santa Rosa CityBus</t>
-  </si>
-  <si>
-    <t>NTD.mode</t>
-  </si>
-  <si>
-    <t>MB</t>
-  </si>
-  <si>
-    <t>CB</t>
-  </si>
-  <si>
-    <t>RB</t>
-  </si>
-  <si>
-    <t>CR</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>LR</t>
-  </si>
-  <si>
-    <t>MG</t>
-  </si>
-  <si>
-    <t>FB</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Napa Vine</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1146,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4847161" cy="609013"/>
     <xdr:sp macro="" textlink="">
@@ -1201,7 +1165,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8924925" y="266700"/>
+          <a:off x="7381875" y="390525"/>
           <a:ext cx="4847161" cy="609013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1252,7 +1216,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Common.Agency.Name and NTD.mode is useful for NTD  correspondence</a:t>
+            <a:t>Common.Agency.Name is useful for NTD </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -2406,11 +2370,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2422,7 +2386,7 @@
     <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>157</v>
       </c>
@@ -2435,1329 +2399,1171 @@
       <c r="D1" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>70</v>
+        <v>114</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
-        <v>6</v>
+        <v>133</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
-        <v>10</v>
+        <v>121</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
-        <v>11</v>
+        <v>130</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>80</v>
+        <v>119</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
+        <v>88</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>101</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>102</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>103</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
         <v>17</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B20" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="18">
-        <v>18</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="18">
-        <v>19</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="18">
-        <v>20</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="18">
-        <v>21</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>88</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
+        <v>113</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="18">
+        <v>114</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="18">
+        <v>115</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="18">
+        <v>116</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="18">
+        <v>117</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="18">
+        <v>131</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="18">
+        <v>132</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="18">
+        <v>134</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="18">
+        <v>136</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="18">
+        <v>137</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="18">
+        <v>68</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="18">
+        <v>24</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="18">
         <v>80</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B55" s="18" t="s">
         <v>111</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="18">
-        <v>81</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="18">
-        <v>82</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E45" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="18">
-        <v>83</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="18">
-        <v>84</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E47" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="18">
-        <v>85</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="E48" s="18" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="18">
-        <v>86</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="E49" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="18">
-        <v>87</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="18">
-        <v>88</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E51" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="18">
-        <v>89</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E52" s="18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="18">
-        <v>90</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="E53" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="18">
-        <v>91</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="E54" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="18">
-        <v>92</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>125</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>112</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="E55" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C56" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="18">
+        <v>20</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="18">
+        <v>21</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="18">
+        <v>89</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="18">
+        <v>110</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="18">
+        <v>135</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="18">
+        <v>58</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="18">
+        <v>49</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="18">
+        <v>91</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D56" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="18">
+      <c r="D64" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="18">
+        <v>63</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="18">
+        <v>1</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="18">
+        <v>2</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="18">
+        <v>3</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="18">
+        <v>4</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="18">
+        <v>5</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="18">
+        <v>6</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="18">
+        <v>7</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="18">
+        <v>44</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="18">
+        <v>38</v>
+      </c>
+      <c r="B74" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C57" s="18" t="s">
+      <c r="C74" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="18">
+        <v>56</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="18">
+        <v>15</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="18">
+        <v>27</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="18">
+        <v>28</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="18">
+        <v>81</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C79" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D57" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="18">
-        <v>95</v>
-      </c>
-      <c r="B58" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="C58" s="18" t="s">
+      <c r="D79" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="18">
+        <v>111</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="18">
+        <v>46</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="18">
+        <v>90</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D58" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="E58" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="18">
-        <v>98</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="18">
+      <c r="D82" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="18">
         <v>100</v>
       </c>
-      <c r="B60" s="18" t="s">
+      <c r="B83" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="C60" s="18" t="s">
+      <c r="C83" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D60" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="18">
-        <v>101</v>
-      </c>
-      <c r="B61" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="C61" s="18" t="s">
+      <c r="D83" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="18">
+        <v>104</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C84" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="D61" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E61" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="18">
-        <v>102</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E62" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="18">
-        <v>103</v>
-      </c>
-      <c r="B63" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D63" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="E63" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="18">
-        <v>104</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="E64" s="18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" s="18">
-        <v>105</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" s="18">
-        <v>106</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="18">
-        <v>110</v>
-      </c>
-      <c r="B67" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E67" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="18">
-        <v>111</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="E68" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="18">
-        <v>112</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D69" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="18">
-        <v>113</v>
-      </c>
-      <c r="B70" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" s="18">
-        <v>114</v>
-      </c>
-      <c r="B71" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C71" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="18">
-        <v>115</v>
-      </c>
-      <c r="B72" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="18">
-        <v>116</v>
-      </c>
-      <c r="B73" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="18">
-        <v>117</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D74" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" s="18">
-        <v>120</v>
-      </c>
-      <c r="B75" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="C75" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D75" s="18" t="s">
+      <c r="D84" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="E75" s="18" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="18">
-        <v>121</v>
-      </c>
-      <c r="B76" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D76" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="E76" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="18">
-        <v>130</v>
-      </c>
-      <c r="B77" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D77" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="E77" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="18">
-        <v>131</v>
-      </c>
-      <c r="B78" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="C78" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D78" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="18">
-        <v>132</v>
-      </c>
-      <c r="B79" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C79" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D79" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="18">
-        <v>133</v>
-      </c>
-      <c r="B80" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="C80" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D80" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E80" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" s="18">
-        <v>134</v>
-      </c>
-      <c r="B81" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D81" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" s="18">
-        <v>135</v>
-      </c>
-      <c r="B82" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C82" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D82" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="E82" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" s="18">
-        <v>136</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C83" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D83" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" s="18">
-        <v>137</v>
-      </c>
-      <c r="B84" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="C84" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D84" s="18" t="s">
-        <v>162</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E84" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
-      <sortCondition ref="A1:A84"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D84">
     <sortCondition ref="D1:D84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge pull request #62 from BayAreaMetro/v1.6_develop""
This reverts commit 672e96801055ca85b30a0ad13fe862ce82de135b.
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one-v1.6_develop\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5D06D0-EACE-4B13-9ABB-FF2A7B3D1A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCC442B-0D1B-4842-82F2-9DF9B7EA09A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="5295" windowWidth="28800" windowHeight="17235" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="285" yWindow="2175" windowWidth="28800" windowHeight="15435" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="County" sheetId="6" r:id="rId6"/>
     <sheet name="Transit Mode" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Transit Mode'!$A$1:$E$84</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="192">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -563,9 +566,6 @@
     <t>FAST</t>
   </si>
   <si>
-    <t>Napa VINE</t>
-  </si>
-  <si>
     <t>Marin Transit</t>
   </si>
   <si>
@@ -585,6 +585,42 @@
   </si>
   <si>
     <t>Union City Transit*</t>
+  </si>
+  <si>
+    <t>Santa Rosa CityBus</t>
+  </si>
+  <si>
+    <t>NTD.mode</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Napa Vine</t>
   </si>
 </sst>
 </file>
@@ -1146,10 +1182,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4847161" cy="609013"/>
     <xdr:sp macro="" textlink="">
@@ -1165,7 +1201,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7381875" y="390525"/>
+          <a:off x="8924925" y="266700"/>
           <a:ext cx="4847161" cy="609013"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1216,7 +1252,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Common.Agency.Name is useful for NTD </a:t>
+            <a:t>Common.Agency.Name and NTD.mode is useful for NTD  correspondence</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -2370,11 +2406,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2386,7 +2422,7 @@
     <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>157</v>
       </c>
@@ -2399,1171 +2435,1329 @@
       <c r="D1" s="18" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>10</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="18">
-        <v>82</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="18">
-        <v>83</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="18">
-        <v>84</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="18">
-        <v>85</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="18">
-        <v>133</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="18">
-        <v>120</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="18">
-        <v>121</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>145</v>
-      </c>
       <c r="D9" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
-        <v>130</v>
+        <v>11</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>147</v>
+        <v>78</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
+        <v>16</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
+        <v>17</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
+        <v>18</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
+        <v>19</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
+        <v>20</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="18">
+      <c r="C19" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
+        <v>21</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="18">
-        <v>101</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="18">
-        <v>102</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="18">
-        <v>103</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="18">
-        <v>17</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
+        <v>30</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
+        <v>33</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="18">
-        <v>95</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>159</v>
-      </c>
       <c r="C25" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
+        <v>80</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="18">
+        <v>81</v>
+      </c>
+      <c r="B44" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="18">
+      <c r="C44" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="18">
+        <v>82</v>
+      </c>
+      <c r="B45" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="18">
+      <c r="C45" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="18">
+        <v>83</v>
+      </c>
+      <c r="B46" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B45" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="18">
+      <c r="C46" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E46" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="18">
+        <v>84</v>
+      </c>
+      <c r="B47" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="18">
+      <c r="C47" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="18">
+        <v>85</v>
+      </c>
+      <c r="B48" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B47" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="18">
-        <v>131</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="C48" s="18" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>150</v>
+        <v>119</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>112</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="B56" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="18">
+        <v>94</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="18">
+        <v>95</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="18">
+        <v>98</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="18">
+        <v>100</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="18">
+        <v>101</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="18">
+        <v>102</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="18">
+        <v>103</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="18">
+        <v>104</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="E64" s="18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="18">
         <v>105</v>
       </c>
-      <c r="C56" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="18">
-        <v>20</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D57" s="18" t="s">
+      <c r="B65" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="18">
+        <v>106</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="18">
+        <v>110</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" s="18" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="18">
-        <v>21</v>
-      </c>
-      <c r="B58" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="18">
-        <v>89</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="18">
-        <v>110</v>
-      </c>
-      <c r="B60" s="18" t="s">
+      <c r="E67" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="18">
+        <v>111</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="18">
+        <v>112</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="18">
+        <v>113</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="18">
+        <v>114</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="18">
+        <v>115</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="18">
+        <v>116</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="18">
+        <v>117</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="18">
+        <v>120</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E75" s="18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="18">
+        <v>121</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="18">
+        <v>130</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E77" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="18">
+        <v>131</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="18">
+        <v>132</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="18">
+        <v>133</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E80" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="18">
+        <v>134</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="18">
+        <v>135</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E82" s="18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="18">
         <v>136</v>
       </c>
-      <c r="C60" s="18" t="s">
+      <c r="B83" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="18">
         <v>137</v>
       </c>
-      <c r="D60" s="18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="18">
-        <v>135</v>
-      </c>
-      <c r="B61" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C61" s="18" t="s">
+      <c r="B84" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C84" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="D61" s="18" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="18">
-        <v>58</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="18">
-        <v>49</v>
-      </c>
-      <c r="B63" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D63" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="18">
-        <v>91</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="18">
-        <v>63</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="18">
-        <v>1</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="18">
-        <v>2</v>
-      </c>
-      <c r="B67" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="18">
-        <v>3</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="18">
-        <v>4</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D69" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="18">
-        <v>5</v>
-      </c>
-      <c r="B70" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="18">
-        <v>6</v>
-      </c>
-      <c r="B71" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="18">
-        <v>7</v>
-      </c>
-      <c r="B72" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="18">
-        <v>44</v>
-      </c>
-      <c r="B73" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="18">
-        <v>38</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D74" s="18" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="18">
-        <v>56</v>
-      </c>
-      <c r="B75" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="C75" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D75" s="18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="18">
-        <v>15</v>
-      </c>
-      <c r="B76" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D76" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="18">
-        <v>27</v>
-      </c>
-      <c r="B77" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D77" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="18">
-        <v>28</v>
-      </c>
-      <c r="B78" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C78" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D78" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="18">
-        <v>81</v>
-      </c>
-      <c r="B79" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C79" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D79" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="18">
-        <v>111</v>
-      </c>
-      <c r="B80" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="C80" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D80" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="18">
-        <v>46</v>
-      </c>
-      <c r="B81" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D81" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="18">
-        <v>90</v>
-      </c>
-      <c r="B82" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C82" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D82" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="18">
-        <v>100</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="C83" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="D83" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="18">
-        <v>104</v>
-      </c>
-      <c r="B84" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="C84" s="18" t="s">
-        <v>129</v>
-      </c>
       <c r="D84" s="18" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D84">
+  <autoFilter ref="A1:E84" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
+      <sortCondition ref="A1:A84"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
     <sortCondition ref="D1:D84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add transit mode 107
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\travel-model-one-v1.6_develop\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCC442B-0D1B-4842-82F2-9DF9B7EA09A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864161DB-7C57-4AB0-B158-56DEE3A56CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="2175" windowWidth="28800" windowHeight="15435" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="3165" yWindow="3105" windowWidth="28800" windowHeight="15435" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Transit Mode" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Transit Mode'!$A$1:$E$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Transit Mode'!$A$1:$E$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="193">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -621,6 +621,9 @@
   </si>
   <si>
     <t>Napa Vine</t>
+  </si>
+  <si>
+    <t>Treasure Island Ferry</t>
   </si>
 </sst>
 </file>
@@ -1268,9 +1271,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1308,7 +1311,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1414,7 +1417,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1556,7 +1559,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2406,11 +2409,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3461,7 +3464,10 @@
         <v>129</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>162</v>
+        <v>175</v>
+      </c>
+      <c r="E65" s="18" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -3480,33 +3486,33 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="18">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>136</v>
+        <v>192</v>
       </c>
       <c r="C67" s="18" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="18">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C68" s="18" t="s">
         <v>137</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>187</v>
@@ -3514,24 +3520,27 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="18">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>137</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
+      </c>
+      <c r="E69" s="18" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="18">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="C70" s="18" t="s">
         <v>137</v>
@@ -3542,10 +3551,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="18">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C71" s="18" t="s">
         <v>137</v>
@@ -3556,10 +3565,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="18">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>137</v>
@@ -3570,10 +3579,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="18">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>137</v>
@@ -3584,10 +3593,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="18">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C74" s="18" t="s">
         <v>137</v>
@@ -3598,27 +3607,24 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="18">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="E75" s="18" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="18">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C76" s="18" t="s">
         <v>145</v>
@@ -3627,46 +3633,49 @@
         <v>176</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="18">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>147</v>
+        <v>176</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="18">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C78" s="18" t="s">
         <v>148</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>162</v>
+        <v>147</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="18">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C79" s="18" t="s">
         <v>148</v>
@@ -3677,72 +3686,72 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="18">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>148</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E80" s="18" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="18">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C81" s="18" t="s">
         <v>148</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>162</v>
+        <v>151</v>
+      </c>
+      <c r="E81" s="18" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="18">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C82" s="18" t="s">
         <v>148</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="E82" s="18" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="18">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C83" s="18" t="s">
         <v>148</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>162</v>
+        <v>153</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="18">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C84" s="18" t="s">
         <v>148</v>
@@ -3751,14 +3760,28 @@
         <v>162</v>
       </c>
     </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="18">
+        <v>137</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E84" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
-      <sortCondition ref="A1:A84"/>
+  <autoFilter ref="A1:E85" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E85">
+      <sortCondition ref="A1:A85"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E84">
-    <sortCondition ref="D1:D84"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E85">
+    <sortCondition ref="D1:D85"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update for Feb 2025 data
And fix bug in Daily VRM Line chart in Tableau
</commit_message>
<xml_diff>
--- a/utilities/TableauAliases.xlsx
+++ b/utilities/TableauAliases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864161DB-7C57-4AB0-B158-56DEE3A56CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187D987F-9424-4D11-A67D-018ED34E3F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="3105" windowWidth="28800" windowHeight="15435" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21570" windowHeight="12870" firstSheet="2" activeTab="6" xr2:uid="{4F82FEDC-82BB-404F-AFFA-9782A7DBBA1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip Mode" sheetId="1" r:id="rId1"/>
@@ -44,8 +44,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={43030453-D6EC-4B92-B8A6-8DD6D9A85C37}</author>
+  </authors>
+  <commentList>
+    <comment ref="A86" authorId="0" shapeId="0" xr:uid="{43030453-D6EC-4B92-B8A6-8DD6D9A85C37}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not modeled. https://www.sonomamarintrain.org/node/543</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="195">
   <si>
     <t>Trip Mode</t>
   </si>
@@ -624,13 +642,19 @@
   </si>
   <si>
     <t>Treasure Island Ferry</t>
+  </si>
+  <si>
+    <t>SMART Connect</t>
+  </si>
+  <si>
+    <t>DR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,6 +709,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1270,6 +1300,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Lisa Zorn" id="{2B3421D1-34F3-4060-BD39-E5CA43D712E2}" userId="S::lzorn@bayareametro.gov::566f6297-4bb7-41af-ba02-cd2b8ef4a845" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1565,6 +1601,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A86" dT="2025-05-01T00:40:00.07" personId="{2B3421D1-34F3-4060-BD39-E5CA43D712E2}" id="{43030453-D6EC-4B92-B8A6-8DD6D9A85C37}">
+    <text>Not modeled. https://www.sonomamarintrain.org/node/543</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>205093859</xltc2:checksum>
+        <xltc2:hyperlink startIndex="13" length="41" url="https://www.sonomamarintrain.org/node/543"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63FD165-F71D-4EB2-B26F-FF4B1D5E4E9C}">
   <dimension ref="A1:B22"/>
@@ -2408,12 +2458,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
-  <dimension ref="A1:E85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3774,6 +3824,23 @@
         <v>162</v>
       </c>
     </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="18">
+        <v>-1</v>
+      </c>
+      <c r="B86" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E85" xr:uid="{5E2C625E-7C69-4E23-869F-A19290811D49}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E85">
@@ -3785,5 +3852,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>